<commit_message>
Fast fertig, kleine Unklarheit im zweiten Teil der Auswertung
</commit_message>
<xml_diff>
--- a/rpm3920.xlsx
+++ b/rpm3920.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desktop\Physik\Grundpraktikum 2\US3---Dopplersonographie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50D0761-E82A-4837-AF4E-10D8217084FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C68C0BF-12A4-4858-8145-09A793BC61FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{9335C19C-04A2-4263-BCB8-10BF28D7C061}"/>
+    <workbookView xWindow="540" yWindow="3810" windowWidth="21600" windowHeight="11295" xr2:uid="{9335C19C-04A2-4263-BCB8-10BF28D7C061}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">Tiefe </t>
-  </si>
-  <si>
     <t>v in cm/s</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>Tiefe</t>
+  </si>
+  <si>
+    <t>Tiefe in mysec</t>
   </si>
 </sst>
 </file>
@@ -409,26 +409,26 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -436,7 +436,8 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>13.2</v>
+        <f>(A2-12.28)*6/4</f>
+        <v>-0.41999999999999904</v>
       </c>
       <c r="C2">
         <v>13.2</v>
@@ -455,13 +456,14 @@
         <v>12.5</v>
       </c>
       <c r="B3">
-        <v>11.5</v>
+        <f t="shared" ref="B3:B17" si="0">(A3-12.28)*6/4</f>
+        <v>0.33000000000000096</v>
       </c>
       <c r="C3">
         <v>11.5</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D17" si="0">C3/100</f>
+        <f t="shared" ref="D3:D17" si="1">C3/100</f>
         <v>0.115</v>
       </c>
       <c r="E3">
@@ -470,17 +472,18 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A16" si="1">A3+0.5</f>
+        <f t="shared" ref="A4:A16" si="2">A3+0.5</f>
         <v>13</v>
       </c>
       <c r="B4">
-        <v>13.2</v>
+        <f t="shared" si="0"/>
+        <v>1.080000000000001</v>
       </c>
       <c r="C4">
         <v>13.2</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13200000000000001</v>
       </c>
       <c r="E4">
@@ -489,17 +492,18 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.5</v>
       </c>
       <c r="B5">
-        <v>14.8</v>
+        <f t="shared" si="0"/>
+        <v>1.830000000000001</v>
       </c>
       <c r="C5">
         <v>14.8</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14800000000000002</v>
       </c>
       <c r="E5">
@@ -508,17 +512,18 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="B6">
-        <v>14.8</v>
+        <f t="shared" si="0"/>
+        <v>2.580000000000001</v>
       </c>
       <c r="C6">
         <v>14.8</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14800000000000002</v>
       </c>
       <c r="E6">
@@ -527,17 +532,18 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.5</v>
       </c>
       <c r="B7">
-        <v>16.5</v>
+        <f t="shared" si="0"/>
+        <v>3.330000000000001</v>
       </c>
       <c r="C7">
         <v>16.5</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E7">
@@ -546,17 +552,18 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="B8">
-        <v>16.5</v>
+        <f t="shared" si="0"/>
+        <v>4.080000000000001</v>
       </c>
       <c r="C8">
         <v>16.5</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E8">
@@ -565,17 +572,18 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.5</v>
       </c>
       <c r="B9">
-        <v>16.5</v>
+        <f t="shared" si="0"/>
+        <v>4.830000000000001</v>
       </c>
       <c r="C9">
         <v>16.5</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E9">
@@ -584,19 +592,19 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="B10">
-        <f>B9</f>
-        <v>16.5</v>
+        <f t="shared" si="0"/>
+        <v>5.580000000000001</v>
       </c>
       <c r="C10">
         <f>C9</f>
         <v>16.5</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E10">
@@ -605,19 +613,19 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.5</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:C15" si="2">B10</f>
-        <v>16.5</v>
+        <f t="shared" si="0"/>
+        <v>6.330000000000001</v>
       </c>
       <c r="C11">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B11:C15" si="3">C10</f>
         <v>16.5</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E11">
@@ -626,19 +634,19 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="B12">
-        <f t="shared" si="2"/>
-        <v>16.5</v>
+        <f t="shared" si="0"/>
+        <v>7.080000000000001</v>
       </c>
       <c r="C12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.5</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E12">
@@ -647,19 +655,19 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="B13">
-        <f t="shared" si="2"/>
-        <v>16.5</v>
+        <f t="shared" si="0"/>
+        <v>7.830000000000001</v>
       </c>
       <c r="C13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.5</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E13">
@@ -668,19 +676,19 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B14">
-        <f t="shared" si="2"/>
-        <v>16.5</v>
+        <f t="shared" si="0"/>
+        <v>8.5800000000000018</v>
       </c>
       <c r="C14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.5</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E14">
@@ -689,19 +697,19 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.5</v>
       </c>
       <c r="B15">
-        <f t="shared" si="2"/>
-        <v>16.5</v>
+        <f t="shared" si="0"/>
+        <v>9.3300000000000018</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.5</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16500000000000001</v>
       </c>
       <c r="E15">
@@ -710,17 +718,18 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B16">
-        <v>14.8</v>
+        <f t="shared" si="0"/>
+        <v>10.080000000000002</v>
       </c>
       <c r="C16">
         <v>14.8</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14800000000000002</v>
       </c>
       <c r="E16">
@@ -733,13 +742,14 @@
         <v>19.5</v>
       </c>
       <c r="B17">
-        <v>14.8</v>
+        <f t="shared" si="0"/>
+        <v>10.830000000000002</v>
       </c>
       <c r="C17">
         <v>14.8</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.14800000000000002</v>
       </c>
       <c r="E17">

</xml_diff>